<commit_message>
atualização planilha de requisitos incluindo tabela Fibonacci
</commit_message>
<xml_diff>
--- a/Gestão/REQUISITOS.xlsx
+++ b/Gestão/REQUISITOS.xlsx
@@ -574,6 +574,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,18 +611,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1767,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,7 +1776,7 @@
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="73.7109375" customWidth="1"/>
     <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="21" style="33" customWidth="1"/>
+    <col min="4" max="4" width="21" style="24" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" customWidth="1"/>
@@ -1798,11 +1798,11 @@
       <c r="E1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="26"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1814,35 +1814,35 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="24">
         <v>13</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="28"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="27"/>
       <c r="I3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="30"/>
+      <c r="K3" s="34"/>
     </row>
     <row r="4" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -1854,16 +1854,16 @@
       <c r="C4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="24">
         <v>13</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="J4" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="32"/>
+      <c r="K4" s="36"/>
     </row>
     <row r="5" spans="1:11" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1875,16 +1875,16 @@
       <c r="C5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="24">
         <v>5</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="32"/>
+      <c r="K5" s="36"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
@@ -1896,7 +1896,7 @@
       <c r="C6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="24">
         <v>13</v>
       </c>
     </row>
@@ -1910,7 +1910,7 @@
       <c r="C7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="24">
         <v>8</v>
       </c>
     </row>
@@ -1924,7 +1924,7 @@
       <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="24">
         <v>3</v>
       </c>
     </row>
@@ -1938,7 +1938,7 @@
       <c r="C9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="24">
         <v>3</v>
       </c>
     </row>
@@ -1952,7 +1952,7 @@
       <c r="C10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="24">
         <v>3</v>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
       <c r="C11" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="24">
         <v>8</v>
       </c>
     </row>
@@ -1980,7 +1980,7 @@
       <c r="C12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="24">
         <v>3</v>
       </c>
     </row>
@@ -1994,7 +1994,7 @@
       <c r="C13" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2008,7 +2008,7 @@
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2022,7 +2022,7 @@
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2036,7 +2036,7 @@
       <c r="C16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2050,7 +2050,7 @@
       <c r="C17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2064,7 +2064,7 @@
       <c r="C18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2078,7 +2078,7 @@
       <c r="C19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="24">
         <v>8</v>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       <c r="C21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2111,7 +2111,7 @@
       <c r="C22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2125,7 +2125,7 @@
       <c r="C23" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="24">
         <v>5</v>
       </c>
     </row>
@@ -2139,7 +2139,7 @@
       <c r="C24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2153,7 +2153,7 @@
       <c r="C25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="33">
+      <c r="D25" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       <c r="C26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="33">
+      <c r="D26" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
       <c r="C27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="24">
         <v>5</v>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
       <c r="C28" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="33">
+      <c r="D28" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
       <c r="C29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="33">
+      <c r="D29" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2223,7 +2223,7 @@
       <c r="C30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="33">
+      <c r="D30" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       <c r="C31" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="33">
+      <c r="D31" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2251,7 +2251,7 @@
       <c r="C32" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="33">
+      <c r="D32" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
       <c r="C33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="33">
+      <c r="D33" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2279,7 +2279,7 @@
       <c r="C34" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="33">
+      <c r="D34" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2293,7 +2293,7 @@
       <c r="C35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="33">
+      <c r="D35" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       <c r="C36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="33">
+      <c r="D36" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       <c r="C37" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="33">
+      <c r="D37" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2335,7 +2335,7 @@
       <c r="C38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="33">
+      <c r="D38" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       <c r="C39" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="33">
+      <c r="D39" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2363,7 +2363,7 @@
       <c r="C40" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="33">
+      <c r="D40" s="24">
         <v>13</v>
       </c>
     </row>
@@ -2377,7 +2377,7 @@
       <c r="C41" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="33">
+      <c r="D41" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       <c r="C42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="33">
+      <c r="D42" s="24">
         <v>5</v>
       </c>
     </row>
@@ -2405,7 +2405,7 @@
       <c r="C43" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="33">
+      <c r="D43" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2419,7 +2419,7 @@
       <c r="C44" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="33">
+      <c r="D44" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       <c r="C45" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="33">
+      <c r="D45" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2447,7 +2447,7 @@
       <c r="C46" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="33">
+      <c r="D46" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
       <c r="C48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="33">
+      <c r="D48" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2480,7 +2480,7 @@
       <c r="C49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="33">
+      <c r="D49" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2494,7 +2494,7 @@
       <c r="C50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="33">
+      <c r="D50" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2508,7 +2508,7 @@
       <c r="C51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="33">
+      <c r="D51" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2522,7 +2522,7 @@
       <c r="C52" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="33">
+      <c r="D52" s="24">
         <v>3</v>
       </c>
     </row>

</xml_diff>